<commit_message>
Updated PreDispatcher Flow with Log Comments
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev2Mercury\Documents\UiPath\InPwr.Finance.AccountsPayable.Common.PreDispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev5pegasus\Documents\Configuration\PreDispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3156235E-7B01-4538-B1C6-069F9B908382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C2F080-DE97-4F8E-8588-84FF6B0D6B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -265,21 +265,6 @@
     <t>@inpwrinc.com</t>
   </si>
   <si>
-    <t>Unable to determine source vendor from email domain.</t>
-  </si>
-  <si>
-    <t>Email domain is Excluded.</t>
-  </si>
-  <si>
-    <t>Mail Subject is empty hence unable to fetch vendor name.</t>
-  </si>
-  <si>
-    <t>Unable to determine source vendor from email subject line.</t>
-  </si>
-  <si>
-    <t>Email Subject is Excluded.</t>
-  </si>
-  <si>
     <t>AP_O365_MailAccount</t>
   </si>
   <si>
@@ -328,21 +313,9 @@
     <t>AP_DataService_FieldName_VendorName</t>
   </si>
   <si>
-    <t>AP_ExceptionLogMessage_Domain</t>
-  </si>
-  <si>
     <t>AP_ExceptionLogMessage_DomainExcluded</t>
   </si>
   <si>
-    <t>AP_ExceptionLogMessage_SubjectMissed</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_Subject</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_SubjectExcluded</t>
-  </si>
-  <si>
     <t>AP_MailValidation_InPwrDomainName</t>
   </si>
   <si>
@@ -388,12 +361,6 @@
     <t>AP_SharedDrive_MappingScript_Flag</t>
   </si>
   <si>
-    <t>AP_KillApplication_Collection</t>
-  </si>
-  <si>
-    <t>EXCEL|msedge</t>
-  </si>
-  <si>
     <t>AP_SharedDrive_UNC</t>
   </si>
   <si>
@@ -511,9 +478,6 @@
     <t>^(?i)(.*?)(?=__?invoice)</t>
   </si>
   <si>
-    <t>C:\RPA\</t>
-  </si>
-  <si>
     <t>Input Folder Name where mails has to be picked</t>
   </si>
   <si>
@@ -533,9 +497,6 @@
   </si>
   <si>
     <t>Dispatcher Queue folder name</t>
-  </si>
-  <si>
-    <t>Kill Process in the Initial stage</t>
   </si>
   <si>
     <t>List of Vendor Types (AP Invoice Process)</t>
@@ -574,10 +535,52 @@
     <t>TEMP;OH_RENT;OH_SWEEP;OH_GENERAL;PO_MATERIAL;PO_SubContractor;PO_Equipment</t>
   </si>
   <si>
-    <t>FinanceAPVendorMasterList;FinanceAPVendorMasterListOH;FinanceAPVendorMasterListPOSC;FinanceAPVendorMasterListPOMaterial;FinanceAPVendorMasterListPOEQ</t>
-  </si>
-  <si>
     <t>\\automationsvr\automation</t>
+  </si>
+  <si>
+    <t>FinanceAPVendorMasterList;FinanceAPVendorMasterListOH</t>
+  </si>
+  <si>
+    <t>Unknown Vendor</t>
+  </si>
+  <si>
+    <t>Vendor is Excluded</t>
+  </si>
+  <si>
+    <t>Subject Line Format error</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_EmptySubject</t>
+  </si>
+  <si>
+    <t>Mail Subject is Empty</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_InvalidSubject</t>
+  </si>
+  <si>
+    <t>Invalid Subject</t>
+  </si>
+  <si>
+    <t>C:</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_InvalidAttachment</t>
+  </si>
+  <si>
+    <t>Mail does not have PDF Attachment</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_DomainNotFound</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_VendorExcluded</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_SubjectFormat</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_VendorNotFound</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -681,9 +684,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,507 +999,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y991"/>
+  <dimension ref="A1:Y994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="122" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56" style="17" customWidth="1"/>
-    <col min="4" max="25" width="8.7109375" style="17" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="17"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:25">
-      <c r="C3" s="18"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" s="17" t="s">
-        <v>148</v>
+      <c r="A4" t="s">
+        <v>137</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="C6" s="18"/>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>167</v>
+      <c r="C7" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="18"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>84</v>
+      <c r="A10" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A11" s="17" t="s">
-        <v>162</v>
+      <c r="A11" t="s">
+        <v>150</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A12" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="B12" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>89</v>
+      <c r="A13" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A14" s="17" t="s">
-        <v>90</v>
+      <c r="A14" t="s">
+        <v>85</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A15" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A16" s="17" t="s">
-        <v>133</v>
+      <c r="A16" t="s">
+        <v>122</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="B17" s="10"/>
-      <c r="C17" s="18"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="17" t="s">
-        <v>118</v>
+      <c r="A18" t="s">
+        <v>109</v>
       </c>
       <c r="B18" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>123</v>
+      <c r="C18" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="17" t="s">
-        <v>124</v>
+      <c r="A19" t="s">
+        <v>113</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>125</v>
+        <v>116</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="17" t="s">
-        <v>126</v>
+      <c r="A20" t="s">
+        <v>115</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>122</v>
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" s="17" t="s">
-        <v>87</v>
+      <c r="A22" t="s">
+        <v>82</v>
       </c>
       <c r="B22" s="11">
         <v>2</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="17" t="s">
-        <v>92</v>
+      <c r="A23" t="s">
+        <v>87</v>
       </c>
       <c r="B23" s="11">
         <v>30</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="18" t="s">
-        <v>93</v>
+      <c r="A24" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>134</v>
+        <v>152</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>94</v>
+      <c r="A25" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>136</v>
+        <v>119</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="18" t="s">
-        <v>95</v>
+      <c r="A26" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>135</v>
+        <v>153</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="17" t="s">
-        <v>106</v>
+      <c r="A27" t="s">
+        <v>97</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>137</v>
+      <c r="C27" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C28" s="18"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>128</v>
+      <c r="A29" t="s">
+        <v>117</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="18"/>
+        <v>173</v>
+      </c>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="18"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="18"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="B31" s="10"/>
-      <c r="C31" s="18"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>96</v>
+      <c r="A32" t="s">
+        <v>91</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>98</v>
+      <c r="A33" t="s">
+        <v>93</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" s="18" t="s">
-        <v>97</v>
+      <c r="A34" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="18" t="s">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="18"/>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="17" t="s">
-        <v>99</v>
+      <c r="A37" t="s">
+        <v>176</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>113</v>
+        <v>166</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>114</v>
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="17" t="s">
-        <v>101</v>
+      <c r="A39" t="s">
+        <v>169</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>112</v>
+        <v>170</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="17" t="s">
-        <v>102</v>
+      <c r="A40" t="s">
+        <v>178</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>115</v>
+        <v>168</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="17" t="s">
-        <v>103</v>
+      <c r="A41" t="s">
+        <v>177</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>116</v>
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="18"/>
+      <c r="A42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" s="12" t="s">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C47" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1">
-      <c r="A44" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="18" t="s">
+    <row r="48" spans="1:3" ht="15" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2438,6 +2446,9 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3662,13 +3673,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>68</v>
@@ -3676,13 +3687,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -3690,13 +3701,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>61</v>
@@ -3704,58 +3715,58 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4775,30 +4786,30 @@
         <v>46</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="210">
       <c r="A3" s="7" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4850,10 +4861,10 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Upgraded as per Exception Log
Upgraded as per Exception Log
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev5pegasus\Documents\Configuration\PreDispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C2F080-DE97-4F8E-8588-84FF6B0D6B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D56D60-2AAA-4AFF-BC77-D95FEFAF6D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="181">
   <si>
     <t>Name</t>
   </si>
@@ -144,12 +144,6 @@
   </si>
   <si>
     <t>EmailTo</t>
-  </si>
-  <si>
-    <t>EmailBcc</t>
-  </si>
-  <si>
-    <t>EmailCc</t>
   </si>
   <si>
     <t>EmailSubject</t>
@@ -259,9 +253,6 @@
     <t>The delay or time interval before retrying the action for the Network share drive.</t>
   </si>
   <si>
-    <t>Regex pattern for Invoice Subject validation.</t>
-  </si>
-  <si>
     <t>@inpwrinc.com</t>
   </si>
   <si>
@@ -319,9 +310,6 @@
     <t>AP_MailValidation_InPwrDomainName</t>
   </si>
   <si>
-    <t>AP_MailValidation_InvoiceSubjectRegex</t>
-  </si>
-  <si>
     <t>AP_SharedDrive_Runtime_SheetName</t>
   </si>
   <si>
@@ -334,9 +322,6 @@
     <t>AP_DataService_RefreshToken</t>
   </si>
   <si>
-    <t>hermes@inpwrinc.com</t>
-  </si>
-  <si>
     <t>Inbox\AP INVOICE ENTRY - CoE\Queued\&lt;VendorType&gt;</t>
   </si>
   <si>
@@ -473,9 +458,6 @@
   </si>
   <si>
     <t>The Asset Name for From period.</t>
-  </si>
-  <si>
-    <t>^(?i)(.*?)(?=__?invoice)</t>
   </si>
   <si>
     <t>Input Folder Name where mails has to be picked</t>
@@ -538,18 +520,12 @@
     <t>\\automationsvr\automation</t>
   </si>
   <si>
-    <t>FinanceAPVendorMasterList;FinanceAPVendorMasterListOH</t>
-  </si>
-  <si>
     <t>Unknown Vendor</t>
   </si>
   <si>
     <t>Vendor is Excluded</t>
   </si>
   <si>
-    <t>Subject Line Format error</t>
-  </si>
-  <si>
     <t>AP_ExceptionLogMessage_EmptySubject</t>
   </si>
   <si>
@@ -559,18 +535,12 @@
     <t>AP_ExceptionLogMessage_InvalidSubject</t>
   </si>
   <si>
-    <t>Invalid Subject</t>
-  </si>
-  <si>
     <t>C:</t>
   </si>
   <si>
     <t>AP_ExceptionLogMessage_InvalidAttachment</t>
   </si>
   <si>
-    <t>Mail does not have PDF Attachment</t>
-  </si>
-  <si>
     <t>AP_ExceptionLogMessage_DomainNotFound</t>
   </si>
   <si>
@@ -581,6 +551,39 @@
   </si>
   <si>
     <t>AP_ExceptionLogMessage_VendorNotFound</t>
+  </si>
+  <si>
+    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\ExceptionLog_Template.xlsx</t>
+  </si>
+  <si>
+    <t>Exception_Log</t>
+  </si>
+  <si>
+    <t>Invalid Subject, [Invoice] Keyword Missing in the Subject.</t>
+  </si>
+  <si>
+    <t>Mail Missing PDF Attachment</t>
+  </si>
+  <si>
+    <t>Subject Line Format Error</t>
+  </si>
+  <si>
+    <t>FinanceAPVendorMasterList;FinanceAPVendorMasterListOH;FinanceAPVendorMasterListPOSC;FinanceAPVendorMasterListPOMaterial</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_ExceptionLog_Template</t>
+  </si>
+  <si>
+    <t>Template for Exception Staging log file path</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_Exception_SheetName</t>
+  </si>
+  <si>
+    <t>AP_MailValidation_InvoiceSubjectRegex</t>
+  </si>
+  <si>
+    <t>^(?i)(.*?)(?=__?invoice)</t>
   </si>
 </sst>
 </file>
@@ -641,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -677,9 +680,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1051,10 +1051,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1062,24 +1062,24 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1087,24 +1087,24 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1114,79 +1114,79 @@
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
@@ -1195,317 +1195,330 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B18" s="11" t="b">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B22" s="11">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" s="11">
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>119</v>
+        <v>176</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>153</v>
+        <v>86</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>70</v>
+      <c r="A27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>147</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C28" s="2"/>
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="10"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B31" s="10"/>
+      <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>164</v>
+      </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>91</v>
+      <c r="A32" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>92</v>
+      <c r="A34" t="s">
+        <v>88</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" t="s">
-        <v>99</v>
+        <v>90</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" t="s">
-        <v>105</v>
-      </c>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
+      </c>
+      <c r="B39" t="s">
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>178</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>168</v>
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
+      </c>
+      <c r="B41" t="s">
+        <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>175</v>
+        <v>160</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>179</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>76</v>
+        <v>163</v>
+      </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3624,7 +3637,7 @@
   <dimension ref="A1:Z976"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3673,100 +3686,100 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4763,7 +4776,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>38</v>
@@ -4772,44 +4785,44 @@
         <v>39</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="240">
       <c r="A2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>157</v>
+        <v>44</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="210">
       <c r="A3" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>157</v>
+        <v>154</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4819,58 +4832,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7C6B43-6EA4-4DD0-939E-D4A6AD374EA2}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="3" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="150">
+    </row>
+    <row r="2" spans="1:4" ht="150">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SET From Period Flag
 Added SET From Period Flag
updated Utility v16
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev5pegasus\Documents\Configuration\PreDispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D56D60-2AAA-4AFF-BC77-D95FEFAF6D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B3399A-384E-47F8-A865-1F67FADF612A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="179">
   <si>
     <t>Name</t>
   </si>
@@ -304,9 +304,6 @@
     <t>AP_DataService_FieldName_VendorName</t>
   </si>
   <si>
-    <t>AP_ExceptionLogMessage_DomainExcluded</t>
-  </si>
-  <si>
     <t>AP_MailValidation_InPwrDomainName</t>
   </si>
   <si>
@@ -326,12 +323,6 @@
   </si>
   <si>
     <t>Exception log message for Subject not found in mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Domain not found in Entity during mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Excluded Domain in Entity during mail validation.</t>
   </si>
   <si>
     <t>Exception log message for Subject not found in Entity during mail validation.</t>
@@ -541,9 +532,6 @@
     <t>AP_ExceptionLogMessage_InvalidAttachment</t>
   </si>
   <si>
-    <t>AP_ExceptionLogMessage_DomainNotFound</t>
-  </si>
-  <si>
     <t>AP_ExceptionLogMessage_VendorExcluded</t>
   </si>
   <si>
@@ -584,6 +572,12 @@
   </si>
   <si>
     <t>^(?i)(.*?)(?=__?invoice)</t>
+  </si>
+  <si>
+    <t>AP_PreDispatcher_FromPeriod_Flag</t>
+  </si>
+  <si>
+    <t>Flagset whether FromPeriod Asset to be updated. "TRUE" to be updated, "FALSE" not to update</t>
   </si>
 </sst>
 </file>
@@ -999,18 +993,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y994"/>
+  <dimension ref="A1:Y992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="122" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="25" width="8.7109375" customWidth="1"/>
+    <col min="4" max="25" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
@@ -1046,68 +1040,68 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="14.5">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" ht="14.5">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" ht="14.5">
       <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="14.5">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="14.5">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" ht="14.5">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="14.5">
+      <c r="A8" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="A8" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="B8" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="14.5">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
@@ -1125,7 +1119,7 @@
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>55</v>
@@ -1142,7 +1136,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>63</v>
@@ -1172,10 +1166,10 @@
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -1183,10 +1177,10 @@
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
@@ -1195,46 +1189,46 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B18" s="11" t="b">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>111</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1264,21 +1258,21 @@
         <v>85</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -1286,10 +1280,10 @@
         <v>86</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1297,29 +1291,29 @@
         <v>87</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1328,19 +1322,19 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -1383,10 +1377,10 @@
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>67</v>
@@ -1397,130 +1391,110 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B39" t="s">
         <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>161</v>
-      </c>
-      <c r="B41" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" t="s">
         <v>168</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" t="s">
-        <v>102</v>
+        <v>162</v>
+      </c>
+      <c r="B43" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
         <v>165</v>
       </c>
-      <c r="B45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>169</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B44" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="A49" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
-        <v>140</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="C52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" t="s">
-        <v>150</v>
-      </c>
-    </row>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2460,8 +2434,6 @@
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2477,12 +2449,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2519,7 +2491,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2530,7 +2502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2644,7 +2616,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3636,16 +3608,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3686,13 +3658,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>66</v>
@@ -3706,7 +3678,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>50</v>
@@ -3720,7 +3692,7 @@
         <v>77</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>59</v>
@@ -3728,44 +3700,44 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3776,13 +3748,26 @@
         <v>80</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4753,6 +4738,7 @@
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4764,17 +4750,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="18.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75">
+    <row r="1" spans="1:5" ht="18.5">
       <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
@@ -4791,7 +4777,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="240">
+    <row r="2" spans="1:5" ht="232">
       <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
@@ -4799,30 +4785,30 @@
         <v>44</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="203">
+      <c r="A3" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="210">
-      <c r="A3" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4838,16 +4824,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="3" width="26.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="18.5">
       <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
@@ -4861,12 +4847,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150">
+    <row r="2" spans="1:4" ht="145">
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Added - Asset status report update component
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev5pegasus\Documents\Configuration\PreDispatcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev2Mercury\Documents\Git\InPwr.Finance.AccountsPayable.Common.PreDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA6C83D-B25F-4231-8233-1893FCDB17D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C040B0-EB4C-46ED-8B00-D33FEFD3C4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -587,6 +587,15 @@
   </si>
   <si>
     <t>AP_DataService_FieldName_SenderAddress</t>
+  </si>
+  <si>
+    <t>AP_StatusReportPath_AssetFolder</t>
+  </si>
+  <si>
+    <t>AP_StatusReportPath_AssetName</t>
+  </si>
+  <si>
+    <t>AP_StatusReportsPath</t>
   </si>
 </sst>
 </file>
@@ -1004,16 +1013,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="122" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="25" width="8.77734375" customWidth="1"/>
+    <col min="4" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
@@ -1049,7 +1058,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="14.4">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1060,10 +1069,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14.4">
+    <row r="3" spans="1:25">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="14.4">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="14.4">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -1085,10 +1094,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="14.4">
+    <row r="6" spans="1:25">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:25" ht="14.4">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="14.4">
+    <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>135</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="14.4">
+    <row r="9" spans="1:25">
       <c r="A9" s="2"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
@@ -1519,8 +1528,22 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A54" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2474,12 +2497,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2516,7 +2539,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2527,7 +2550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2641,7 +2664,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3634,15 +3657,15 @@
   <dimension ref="A1:Z976"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4775,17 +4798,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="7"/>
+    <col min="1" max="1" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
@@ -4802,7 +4825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="230.4">
+    <row r="2" spans="1:5" ht="240">
       <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
@@ -4819,7 +4842,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="201.6">
+    <row r="3" spans="1:5" ht="210">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
@@ -4849,16 +4872,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.21875" style="7"/>
+    <col min="3" max="3" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
@@ -4872,7 +4895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="144">
+    <row r="2" spans="1:4" ht="150">
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>

</xml_diff>